<commit_message>
Added ERD, Updated status report
Added Entity Relationship Diagram. Updated Project Status Report. Minor updates to Data Dictionary.
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b23540b5940dc24b/Documents/GitHub/pet-adoption-platform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="13_ncr:1_{C1B0FE99-43D3-4C83-9A70-446CD0ACE2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAF8741B-1445-4844-9CA9-9935A615CA44}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="13_ncr:1_{C1B0FE99-43D3-4C83-9A70-446CD0ACE2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD9F9781-A8BF-4300-9357-7F4DE54BD66A}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{53CEDAC0-C0B7-4620-9FC4-13FBD529EB5A}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{53CEDAC0-C0B7-4620-9FC4-13FBD529EB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="102">
   <si>
     <t>Entities</t>
   </si>
@@ -210,15 +210,6 @@
   </si>
   <si>
     <t>The name of the file</t>
-  </si>
-  <si>
-    <t>The file type</t>
-  </si>
-  <si>
-    <t>jpg, png</t>
-  </si>
-  <si>
-    <t>The file size in bytes</t>
   </si>
   <si>
     <t>The image height in pixels</t>
@@ -414,14 +405,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +560,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC571A79-7597-4ED5-B7C7-7BAE304AE8C8}" name="Table13" displayName="Table13" ref="A3:I11" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A3:I11" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC571A79-7597-4ED5-B7C7-7BAE304AE8C8}" name="Table13" displayName="Table13" ref="A3:I9" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A3:I9" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{EB709C33-59D5-425D-8377-7248B32C02CE}" name="Column Name"/>
     <tableColumn id="2" xr3:uid="{75254070-CA4E-480C-B2F3-A37C89E13CC5}" name="Data Type"/>
@@ -589,7 +578,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FF2989B8-E871-46A4-954C-1AD070896BFA}" name="Table135" displayName="Table135" ref="A3:I6" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FF2989B8-E871-46A4-954C-1AD070896BFA}" name="Table135" displayName="Table135" ref="A3:I6" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A3:I6" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BC8071A3-E8B8-448C-A6BC-80674C1B3E55}" name="Column Name"/>
@@ -607,7 +596,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2F851650-791A-4B1B-AD76-4200E4AD3FB8}" name="Table134" displayName="Table134" ref="A3:I14" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2F851650-791A-4B1B-AD76-4200E4AD3FB8}" name="Table134" displayName="Table134" ref="A3:I14" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A3:I14" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{481A897D-79ED-4701-A306-8AE478D3E8D1}" name="Column Name"/>
@@ -625,7 +614,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6F585819-CDFC-49F1-B896-89A8E691B468}" name="Table13456" displayName="Table13456" ref="A3:I4" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6F585819-CDFC-49F1-B896-89A8E691B468}" name="Table13456" displayName="Table13456" ref="A3:I4" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A3:I4" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4E0CB051-CCD2-4A85-8D7B-8CA3CCEEF6A0}" name="Column Name"/>
@@ -643,7 +632,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4607B877-37BB-47F2-8507-417D87380272}" name="Table134567" displayName="Table134567" ref="A3:I8" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4607B877-37BB-47F2-8507-417D87380272}" name="Table134567" displayName="Table134567" ref="A3:I8" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A3:I8" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FBEFA340-7F68-401A-9E6D-41F0196FC817}" name="Column Name"/>
@@ -979,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1EB38A2-ED52-43FF-841F-8E6F88246B9B}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -995,10 +984,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1008,7 +997,7 @@
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1019,29 +1008,29 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1052,7 +1041,7 @@
       <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1063,18 +1052,18 @@
       <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1166,7 +1155,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1178,7 +1167,7 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1345,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68F5497-3B2C-49F6-9D76-3F15F3B4A916}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1346,7 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" customWidth="1"/>
+    <col min="7" max="7" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" customWidth="1"/>
   </cols>
@@ -1429,7 +1418,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>500</v>
@@ -1460,12 +1449,9 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
         <v>10</v>
       </c>
       <c r="D7" t="s">
@@ -1474,13 +1460,11 @@
       <c r="G7" t="s">
         <v>56</v>
       </c>
-      <c r="I7" t="s">
-        <v>57</v>
-      </c>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -1489,53 +1473,24 @@
         <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>1000</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1605,25 +1560,21 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1639,12 +1590,12 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1653,10 +1604,10 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1688,12 +1639,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1727,7 +1678,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -1762,10 +1713,10 @@
         <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1782,12 +1733,12 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -1799,12 +1750,12 @@
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1816,12 +1767,12 @@
         <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1833,12 +1784,12 @@
         <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -1850,15 +1801,15 @@
         <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1870,15 +1821,15 @@
         <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -1890,7 +1841,7 @@
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I12">
         <v>5551119876</v>
@@ -1910,7 +1861,7 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1927,7 +1878,7 @@
         <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1964,7 +1915,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1998,7 +1949,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -2053,7 +2004,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2087,7 +2038,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -2110,7 +2061,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2122,12 +2073,12 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -2139,12 +2090,12 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2156,12 +2107,12 @@
         <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -2170,7 +2121,7 @@
         <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>